<commit_message>
Quick tweak to verifymatrix; it erroneously reported matching row & column names.
</commit_message>
<xml_diff>
--- a/inst/extdata/bad_matrix.xlsx
+++ b/inst/extdata/bad_matrix.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\Syncthing-Docs\Dissertation\Scalation Networks\pholidosis\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User1\Syncthing-Docs\Dissertation\Scalation Networks\pholidosis\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DF136B-CC86-4962-8F29-0E4FC44978D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B9E17F-3D8E-4415-856E-3D84908F0B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="2" xr2:uid="{DB39FBCB-727B-45A7-8412-F72E8590918E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{DB39FBCB-727B-45A7-8412-F72E8590918E}"/>
   </bookViews>
   <sheets>
-    <sheet name="bad_names" sheetId="1" r:id="rId1"/>
-    <sheet name="bad_entry" sheetId="3" r:id="rId2"/>
-    <sheet name="fixed" sheetId="4" r:id="rId3"/>
+    <sheet name="m1 - bad_names" sheetId="1" r:id="rId1"/>
+    <sheet name="m2 - bad_entry" sheetId="3" r:id="rId2"/>
+    <sheet name="m3 - not_spherical" sheetId="6" r:id="rId3"/>
+    <sheet name="fixed" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,8 +38,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="37">
   <si>
     <t>R_post-infralabial_3</t>
   </si>
@@ -143,6 +166,12 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>mouth</t>
   </si>
 </sst>
 </file>
@@ -310,9 +339,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -350,7 +379,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -456,7 +485,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -598,7 +627,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3069,12 +3098,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB401DFA-661F-42D2-830D-7C7A2967AC39}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6264BF-8D82-4209-8E40-3B083D403E09}">
   <dimension ref="A1:AG33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V11" sqref="V11"/>
+      <selection pane="topRight" activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4298,4 +4327,1515 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB401DFA-661F-42D2-830D-7C7A2967AC39}">
+  <dimension ref="A1:AI35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I41" sqref="I41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V1" t="s">
+        <v>13</v>
+      </c>
+      <c r="W1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="14"/>
+      <c r="D2" cm="1">
+        <f t="array" ref="D2:AI3">TRANSPOSE(B4:C35)</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>1</v>
+      </c>
+      <c r="AH2">
+        <v>1</v>
+      </c>
+      <c r="AI2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="8"/>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="21">
+        <v>1</v>
+      </c>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14">
+        <v>1</v>
+      </c>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="21">
+        <v>1</v>
+      </c>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="14"/>
+      <c r="AF4" s="14"/>
+      <c r="AG4" s="14"/>
+      <c r="AH4" s="14"/>
+      <c r="AI4" s="13"/>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="8"/>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="9">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="W5" s="9">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="7"/>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="W6" s="9"/>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="AD6">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="7"/>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="J7" s="9"/>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="W7" s="9"/>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AI7" s="7"/>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="H8" s="8"/>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="W8" s="9"/>
+      <c r="AF8">
+        <v>1</v>
+      </c>
+      <c r="AI8" s="7"/>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="20"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2">
+        <v>1</v>
+      </c>
+      <c r="T9" s="2">
+        <v>1</v>
+      </c>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="19"/>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="15"/>
+      <c r="K10" s="14">
+        <v>3</v>
+      </c>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14">
+        <v>3</v>
+      </c>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="12">
+        <v>1</v>
+      </c>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="11"/>
+      <c r="AG10" s="11"/>
+      <c r="AH10" s="11"/>
+      <c r="AI10" s="10"/>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="J11" s="9">
+        <v>3</v>
+      </c>
+      <c r="K11" s="8"/>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="V11" s="7"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="11"/>
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="11"/>
+      <c r="AG11" s="11"/>
+      <c r="AH11" s="11"/>
+      <c r="AI11" s="10"/>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" s="8"/>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="V12" s="7"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="11"/>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="11"/>
+      <c r="AC12" s="11"/>
+      <c r="AD12" s="11"/>
+      <c r="AE12" s="11"/>
+      <c r="AF12" s="11"/>
+      <c r="AG12" s="11"/>
+      <c r="AH12" s="11"/>
+      <c r="AI12" s="10"/>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="J13" s="9">
+        <v>3</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="M13" s="8"/>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="V13" s="7"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="11"/>
+      <c r="AC13" s="11"/>
+      <c r="AD13" s="11"/>
+      <c r="AE13" s="11"/>
+      <c r="AF13" s="11"/>
+      <c r="AG13" s="11"/>
+      <c r="AH13" s="11"/>
+      <c r="AI13" s="10"/>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14" s="8"/>
+      <c r="O14">
+        <v>3</v>
+      </c>
+      <c r="V14" s="7"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="11"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="11"/>
+      <c r="AF14" s="11"/>
+      <c r="AG14" s="11"/>
+      <c r="AH14" s="11"/>
+      <c r="AI14" s="10"/>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>3</v>
+      </c>
+      <c r="O15" s="8"/>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="V15" s="7"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="11"/>
+      <c r="AD15" s="11"/>
+      <c r="AE15" s="11"/>
+      <c r="AF15" s="11"/>
+      <c r="AG15" s="11"/>
+      <c r="AH15" s="11"/>
+      <c r="AI15" s="10"/>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16" s="8"/>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="V16" s="7"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="11"/>
+      <c r="AD16" s="11"/>
+      <c r="AE16" s="11"/>
+      <c r="AF16" s="11"/>
+      <c r="AG16" s="11"/>
+      <c r="AH16" s="11"/>
+      <c r="AI16" s="10"/>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="J17" s="9"/>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="8"/>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="V17" s="7"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="11"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="11"/>
+      <c r="AD17" s="11"/>
+      <c r="AE17" s="11"/>
+      <c r="AF17" s="11"/>
+      <c r="AG17" s="11"/>
+      <c r="AH17" s="11"/>
+      <c r="AI17" s="10"/>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="J18" s="9"/>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18" s="8"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="11"/>
+      <c r="AF18" s="11"/>
+      <c r="AG18" s="11"/>
+      <c r="AH18" s="11"/>
+      <c r="AI18" s="10"/>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19" s="9"/>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="S19" s="8"/>
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="V19" s="7">
+        <v>1</v>
+      </c>
+      <c r="W19" s="12"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="11"/>
+      <c r="AE19" s="11"/>
+      <c r="AF19" s="11"/>
+      <c r="AG19" s="11"/>
+      <c r="AH19" s="11"/>
+      <c r="AI19" s="10"/>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20" s="9"/>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20" s="8"/>
+      <c r="U20">
+        <v>1</v>
+      </c>
+      <c r="V20" s="7"/>
+      <c r="W20" s="12"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="11"/>
+      <c r="AB20" s="11"/>
+      <c r="AC20" s="11"/>
+      <c r="AD20" s="11"/>
+      <c r="AE20" s="11"/>
+      <c r="AF20" s="11"/>
+      <c r="AG20" s="11"/>
+      <c r="AH20" s="11"/>
+      <c r="AI20" s="10"/>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="U21" s="8"/>
+      <c r="V21" s="7">
+        <v>1</v>
+      </c>
+      <c r="W21" s="12"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="11"/>
+      <c r="AD21" s="11"/>
+      <c r="AE21" s="11"/>
+      <c r="AF21" s="11"/>
+      <c r="AG21" s="11"/>
+      <c r="AH21" s="11"/>
+      <c r="AI21" s="10"/>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2">
+        <v>1</v>
+      </c>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2">
+        <v>1</v>
+      </c>
+      <c r="V22" s="1"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5"/>
+      <c r="AC22" s="5"/>
+      <c r="AD22" s="5"/>
+      <c r="AE22" s="5"/>
+      <c r="AF22" s="5"/>
+      <c r="AG22" s="5"/>
+      <c r="AH22" s="5"/>
+      <c r="AI22" s="4"/>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="9">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="J23" s="18">
+        <v>1</v>
+      </c>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="17"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="15"/>
+      <c r="X23" s="14">
+        <v>3</v>
+      </c>
+      <c r="Y23" s="14"/>
+      <c r="Z23" s="14">
+        <v>3</v>
+      </c>
+      <c r="AA23" s="14"/>
+      <c r="AB23" s="14"/>
+      <c r="AC23" s="14"/>
+      <c r="AD23" s="14"/>
+      <c r="AE23" s="14"/>
+      <c r="AF23" s="14"/>
+      <c r="AG23" s="14"/>
+      <c r="AH23" s="14"/>
+      <c r="AI23" s="13"/>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="J24" s="12"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="9">
+        <v>3</v>
+      </c>
+      <c r="X24" s="8"/>
+      <c r="Y24">
+        <v>1</v>
+      </c>
+      <c r="Z24">
+        <v>1</v>
+      </c>
+      <c r="AA24">
+        <v>1</v>
+      </c>
+      <c r="AI24" s="7"/>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="J25" s="12"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="9"/>
+      <c r="X25">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="8"/>
+      <c r="AA25">
+        <v>1</v>
+      </c>
+      <c r="AB25">
+        <v>1</v>
+      </c>
+      <c r="AC25">
+        <v>1</v>
+      </c>
+      <c r="AD25">
+        <v>1</v>
+      </c>
+      <c r="AI25" s="7"/>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="9">
+        <v>1</v>
+      </c>
+      <c r="J26" s="12"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="9">
+        <v>3</v>
+      </c>
+      <c r="X26">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="8"/>
+      <c r="AA26">
+        <v>1</v>
+      </c>
+      <c r="AI26" s="7"/>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="9"/>
+      <c r="X27">
+        <v>1</v>
+      </c>
+      <c r="Y27">
+        <v>1</v>
+      </c>
+      <c r="Z27">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="8"/>
+      <c r="AB27">
+        <v>3</v>
+      </c>
+      <c r="AI27" s="7"/>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="10"/>
+      <c r="W28" s="9"/>
+      <c r="Y28">
+        <v>1</v>
+      </c>
+      <c r="AA28">
+        <v>3</v>
+      </c>
+      <c r="AB28" s="8"/>
+      <c r="AC28">
+        <v>1</v>
+      </c>
+      <c r="AI28" s="7"/>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="10"/>
+      <c r="W29" s="9"/>
+      <c r="Y29">
+        <v>1</v>
+      </c>
+      <c r="AB29">
+        <v>1</v>
+      </c>
+      <c r="AC29" s="8"/>
+      <c r="AD29">
+        <v>1</v>
+      </c>
+      <c r="AF29">
+        <v>1</v>
+      </c>
+      <c r="AI29" s="7"/>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="J30" s="12"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="10"/>
+      <c r="W30" s="9"/>
+      <c r="Y30">
+        <v>1</v>
+      </c>
+      <c r="AC30">
+        <v>1</v>
+      </c>
+      <c r="AD30" s="8"/>
+      <c r="AE30">
+        <v>1</v>
+      </c>
+      <c r="AI30" s="7"/>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="J31" s="12"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="10"/>
+      <c r="W31" s="9"/>
+      <c r="AD31">
+        <v>1</v>
+      </c>
+      <c r="AE31" s="8"/>
+      <c r="AI31" s="7"/>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32" s="12"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="10"/>
+      <c r="W32" s="9"/>
+      <c r="AC32">
+        <v>1</v>
+      </c>
+      <c r="AF32" s="8"/>
+      <c r="AG32">
+        <v>1</v>
+      </c>
+      <c r="AH32">
+        <v>1</v>
+      </c>
+      <c r="AI32" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33" s="12"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="T33" s="11"/>
+      <c r="U33" s="11"/>
+      <c r="V33" s="10"/>
+      <c r="W33" s="9"/>
+      <c r="AF33">
+        <v>1</v>
+      </c>
+      <c r="AG33" s="8"/>
+      <c r="AH33">
+        <v>1</v>
+      </c>
+      <c r="AI33" s="7"/>
+    </row>
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="9"/>
+      <c r="AF34">
+        <v>1</v>
+      </c>
+      <c r="AG34">
+        <v>1</v>
+      </c>
+      <c r="AH34" s="8"/>
+      <c r="AI34" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="5"/>
+      <c r="U35" s="5"/>
+      <c r="V35" s="4"/>
+      <c r="W35" s="3"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
+      <c r="Z35" s="2"/>
+      <c r="AA35" s="2"/>
+      <c r="AB35" s="2"/>
+      <c r="AC35" s="2"/>
+      <c r="AD35" s="2"/>
+      <c r="AE35" s="2"/>
+      <c r="AF35" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG35" s="2"/>
+      <c r="AH35" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI35" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
 </file>
</xml_diff>